<commit_message>
#57 + #58 Initialiserungen und Evaluation des Frontends
</commit_message>
<xml_diff>
--- a/docs/arc42/resources/techevaluationfe.xlsx
+++ b/docs/arc42/resources/techevaluationfe.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/mumaxi2/git/mxmueller/DHBW-Blickbox/docs/arc42/resources/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D4094096-3E9C-304F-9CD3-03AFB0609BCD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4099995B-7956-0748-9DF4-47455B1E5993}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="840" yWindow="780" windowWidth="28240" windowHeight="17240" xr2:uid="{2507937E-729C-CD4F-8100-AAA5900B3C22}"/>
   </bookViews>
@@ -281,16 +281,16 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
@@ -608,17 +608,20 @@
   <dimension ref="A1:I9"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="125" workbookViewId="0">
-      <selection activeCell="F13" sqref="F13"/>
+      <selection activeCell="H10" sqref="H10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="2" max="2" width="9.5" customWidth="1"/>
-    <col min="3" max="3" width="30.83203125" customWidth="1"/>
-    <col min="4" max="4" width="13" customWidth="1"/>
-    <col min="5" max="5" width="14.33203125" customWidth="1"/>
-    <col min="6" max="6" width="13.6640625" customWidth="1"/>
-    <col min="7" max="7" width="13.33203125" customWidth="1"/>
+    <col min="1" max="1" width="30.6640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="12.6640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="7.6640625" customWidth="1"/>
+    <col min="4" max="4" width="8.1640625" customWidth="1"/>
+    <col min="5" max="5" width="7.1640625" customWidth="1"/>
+    <col min="6" max="6" width="7.6640625" customWidth="1"/>
+    <col min="7" max="7" width="6.5" customWidth="1"/>
+    <col min="8" max="8" width="7.33203125" customWidth="1"/>
+    <col min="9" max="9" width="5.83203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:9" ht="19" x14ac:dyDescent="0.25">
@@ -626,21 +629,21 @@
       <c r="B1" s="10" t="s">
         <v>2</v>
       </c>
-      <c r="C1" s="15" t="s">
+      <c r="C1" s="11" t="s">
         <v>1</v>
       </c>
-      <c r="D1" s="16"/>
-      <c r="E1" s="15" t="s">
+      <c r="D1" s="12"/>
+      <c r="E1" s="11" t="s">
         <v>3</v>
       </c>
-      <c r="F1" s="16"/>
-      <c r="G1" s="15" t="s">
+      <c r="F1" s="12"/>
+      <c r="G1" s="11" t="s">
         <v>4</v>
       </c>
-      <c r="H1" s="16"/>
+      <c r="H1" s="12"/>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A2" s="11" t="s">
+      <c r="A2" s="13" t="s">
         <v>8</v>
       </c>
       <c r="B2" s="4">
@@ -669,7 +672,7 @@
       </c>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A3" s="11" t="s">
+      <c r="A3" s="13" t="s">
         <v>9</v>
       </c>
       <c r="B3" s="4">
@@ -698,7 +701,7 @@
       </c>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A4" s="11" t="s">
+      <c r="A4" s="13" t="s">
         <v>0</v>
       </c>
       <c r="B4" s="4">
@@ -727,7 +730,7 @@
       </c>
     </row>
     <row r="5" spans="1:9" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="12" t="s">
+      <c r="A5" s="14" t="s">
         <v>10</v>
       </c>
       <c r="B5" s="5">
@@ -757,7 +760,7 @@
       <c r="I5" s="2"/>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A6" s="13" t="s">
+      <c r="A6" s="15" t="s">
         <v>5</v>
       </c>
       <c r="B6" s="4">
@@ -767,7 +770,7 @@
         <f>SUM(C2:C5)</f>
         <v>317</v>
       </c>
-      <c r="D6" s="14">
+      <c r="D6" s="16">
         <f t="shared" ref="D6:H6" si="3">SUM(D2:D5)</f>
         <v>1145</v>
       </c>
@@ -803,6 +806,11 @@
       </c>
     </row>
   </sheetData>
+  <mergeCells count="3">
+    <mergeCell ref="G1:H1"/>
+    <mergeCell ref="E1:F1"/>
+    <mergeCell ref="C1:D1"/>
+  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="landscape" horizontalDpi="0" verticalDpi="0"/>
 </worksheet>

</xml_diff>